<commit_message>
Allow negative numbers in conditional part of format string
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/FormatConditionTests.xlsx
+++ b/test-data/spreadsheet/FormatConditionTests.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anthonyschott/repos/poi/test-data/spreadsheet/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8FC395-3264-2946-AD52-A6A16AB4BB9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25840" yWindow="-80" windowWidth="10960" windowHeight="22840" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="30140" yWindow="3260" windowWidth="25340" windowHeight="22840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flags" sheetId="2" r:id="rId1"/>
     <sheet name="Tests" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="36">
   <si>
     <t>Run the test with all standard colors specified</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -109,20 +115,49 @@
   <si>
     <t>Categories</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[&lt;-10]#" Wow"</t>
+  </si>
+  <si>
+    <t>[&gt;-10]#" Big"</t>
+  </si>
+  <si>
+    <t>[&lt;=-10]#" Wow"</t>
+  </si>
+  <si>
+    <t>[&gt;=-10]#" Big"</t>
+  </si>
+  <si>
+    <t>[=-10]#" Wow"</t>
+  </si>
+  <si>
+    <t>[&lt;&gt;-10]#" Wow"</t>
+  </si>
+  <si>
+    <t>[&lt; -10]#" Wow"</t>
+  </si>
+  <si>
+    <t>-11 Wow</t>
+  </si>
+  <si>
+    <t>-10</t>
+  </si>
+  <si>
+    <t>-9</t>
+  </si>
+  <si>
+    <t>-10 Wow</t>
+  </si>
+  <si>
+    <t>[&lt;      -10]#" Wow"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -139,6 +174,11 @@
     <font>
       <sz val="10"/>
       <name val="Lucida Sans Typewriter"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Lucida Sans Typewriter"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -167,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -199,7 +239,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -208,6 +254,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -530,7 +584,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -538,15 +592,15 @@
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="7"/>
+    <col min="1" max="1" width="10.6640625" style="7"/>
     <col min="2" max="2" width="17" style="8" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" style="8" customWidth="1"/>
-    <col min="4" max="16384" width="10.7109375" style="1"/>
+    <col min="3" max="3" width="34.83203125" style="8" customWidth="1"/>
+    <col min="4" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -557,7 +611,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="26">
+    <row r="2" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
@@ -565,7 +619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>18</v>
       </c>
@@ -574,7 +628,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
@@ -598,25 +652,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:D341"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H342"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28:XFD29"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="10.7109375" style="2"/>
+    <col min="5" max="16384" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -630,7 +684,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="str">
         <f>TEXT(C2, B2)</f>
         <v>1 Wow</v>
@@ -645,7 +699,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="str">
         <f t="shared" ref="A3:A7" si="0">TEXT(C3, B3)</f>
         <v>10</v>
@@ -660,7 +714,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="str">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -675,7 +729,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -690,7 +744,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="9" t="str">
         <f t="shared" si="0"/>
         <v>11 Big</v>
@@ -705,7 +759,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="9" t="str">
         <f t="shared" si="0"/>
         <v>12 Big</v>
@@ -719,8 +773,9 @@
       <c r="D7" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="H7" s="11"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="9" t="str">
         <f>TEXT(C8, B8)</f>
         <v>1 Wow</v>
@@ -735,7 +790,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="str">
         <f t="shared" ref="A9:A11" si="1">TEXT(C9, B9)</f>
         <v>10 Wow</v>
@@ -750,7 +805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="str">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -765,7 +820,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="str">
         <f t="shared" si="1"/>
         <v>10 Big</v>
@@ -780,7 +835,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="str">
         <f t="shared" ref="A12:A13" si="2">TEXT(C12, B12)</f>
         <v>11 Big</v>
@@ -795,7 +850,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="str">
         <f t="shared" si="2"/>
         <v>12 Big</v>
@@ -810,7 +865,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="str">
         <f>TEXT(C14, B14)</f>
         <v>1</v>
@@ -825,7 +880,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="str">
         <f t="shared" ref="A15:A16" si="3">TEXT(C15, B15)</f>
         <v>10 Wow</v>
@@ -840,7 +895,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="str">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -855,7 +910,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="str">
         <f>TEXT(C17, B17)</f>
         <v>1 Wow</v>
@@ -870,7 +925,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="str">
         <f t="shared" ref="A18:A19" si="4">TEXT(C18, B18)</f>
         <v>10</v>
@@ -885,7 +940,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="9" t="str">
         <f t="shared" si="4"/>
         <v>11 Wow</v>
@@ -900,1148 +955,1336 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="D20" s="7"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="9" t="str">
-        <f>TEXT(C21, B21)</f>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A20" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="12">
+        <v>-11</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A21" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="12">
+        <v>-10</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A22" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="12">
+        <v>-9</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A23" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="12">
+        <v>-10</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A24" s="9" t="str">
+        <f t="shared" ref="A21:A25" si="5">TEXT(C24, B24)</f>
+        <v>-9 Big</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="12">
+        <v>-9</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A25" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>-8 Big</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="12">
+        <v>-8</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A26" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="12">
+        <v>-11</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A27" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="12">
+        <v>-10</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A28" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="12">
+        <v>-9</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A29" s="9" t="str">
+        <f t="shared" ref="A27:A31" si="6">TEXT(C29, B29)</f>
+        <v>-10 Big</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="12">
+        <v>-10</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A30" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v>-9 Big</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="12">
+        <v>-9</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A31" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v>-8 Big</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="12">
+        <v>-8</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A32" s="9" t="str">
+        <f>TEXT(C32, B32)</f>
+        <v>-11</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="12">
+        <v>-11</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A33" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="12">
+        <v>-10</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A34" s="9" t="str">
+        <f t="shared" ref="A33:A34" si="7">TEXT(C34, B34)</f>
+        <v>-9</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="12">
+        <v>-9</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A35" s="9" t="str">
+        <f>TEXT(C35, B35)</f>
+        <v>-11 Wow</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="12">
+        <v>-11</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A36" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="12">
+        <v>-10</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A37" s="9" t="str">
+        <f t="shared" ref="A36:A37" si="8">TEXT(C37, B37)</f>
+        <v>-9 Wow</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="12">
+        <v>-9</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A38" s="9" t="str">
+        <f t="shared" ref="A38:A54" si="9">TEXT(C38, B38)</f>
+        <v/>
+      </c>
+      <c r="D38" s="7"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A39" s="9" t="str">
+        <f>TEXT(C39, B39)</f>
         <v>1 Wow</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B39" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C39" s="2">
         <v>1</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D39" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="9" t="str">
-        <f t="shared" ref="A22" si="5">TEXT(C22, B22)</f>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A40" s="9" t="str">
+        <f t="shared" ref="A40" si="10">TEXT(C40, B40)</f>
         <v>10</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B40" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C40" s="2">
         <v>10</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D40" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="9" t="str">
-        <f>TEXT(C23, B23)</f>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A41" s="9" t="str">
+        <f>TEXT(C41, B41)</f>
         <v>1 Wow</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B41" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C41" s="2">
         <v>1</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D41" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="9" t="str">
-        <f t="shared" ref="A24" si="6">TEXT(C24, B24)</f>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A42" s="9" t="str">
+        <f t="shared" ref="A42" si="11">TEXT(C42, B42)</f>
         <v>10</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B42" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C42" s="2">
         <v>10</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D42" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="9" t="str">
-        <f>TEXT(C25, B25)</f>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A43" s="9" t="str">
+        <f>TEXT(C43, B43)</f>
         <v>1 Wow</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B43" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C43" s="2">
         <v>1</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D43" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="9" t="str">
-        <f t="shared" ref="A26:A53" si="7">TEXT(C26, B26)</f>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A44" s="9" t="str">
+        <f>TEXT(C44, B44)</f>
         <v>10</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B44" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C44" s="2">
         <v>10</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D44" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="9" t="str">
-        <f t="shared" si="7"/>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A45" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="2">
+        <v>-11</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A46" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" s="2">
+        <v>-10</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A47" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" s="2">
+        <v>-11</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A48" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" s="2">
+        <v>-10</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A49" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C49" s="2">
+        <v>-11</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A50" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C50" s="2">
+        <v>-10</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A51" s="9" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="D27" s="7"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="9" t="str">
-        <f t="shared" si="7"/>
+      <c r="D51" s="7"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A52" s="9" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="D28" s="7"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="9" t="str">
-        <f t="shared" si="7"/>
+      <c r="D52" s="7"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A53" s="9" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="D29" s="7"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="9" t="str">
-        <f t="shared" si="7"/>
+      <c r="D53" s="7"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A54" s="9" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="D30" s="7"/>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D31" s="7"/>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D32" s="7"/>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D33" s="7"/>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D34" s="7"/>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="7"/>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D36" s="7"/>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D37" s="7"/>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D38" s="7"/>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D39" s="7"/>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D40" s="7"/>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D41" s="7"/>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D42" s="7"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D43" s="7"/>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D44" s="7"/>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D45" s="7"/>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D46" s="7"/>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D47" s="7"/>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D48" s="7"/>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D49" s="7"/>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D50" s="7"/>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D51" s="7"/>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D52" s="7"/>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D53" s="7"/>
-    </row>
-    <row r="54" spans="1:4">
       <c r="D54" s="7"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D55" s="7"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D56" s="7"/>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D57" s="7"/>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D58" s="7"/>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D59" s="7"/>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D60" s="7"/>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D61" s="7"/>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D62" s="7"/>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D63" s="7"/>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D64" s="7"/>
     </row>
-    <row r="65" spans="4:4">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D65" s="7"/>
     </row>
-    <row r="66" spans="4:4">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D66" s="7"/>
     </row>
-    <row r="67" spans="4:4">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D67" s="7"/>
     </row>
-    <row r="68" spans="4:4">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D68" s="7"/>
     </row>
-    <row r="69" spans="4:4">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D69" s="7"/>
     </row>
-    <row r="70" spans="4:4">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D70" s="7"/>
     </row>
-    <row r="71" spans="4:4">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D71" s="7"/>
     </row>
-    <row r="72" spans="4:4">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D72" s="7"/>
     </row>
-    <row r="73" spans="4:4">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D73" s="7"/>
     </row>
-    <row r="74" spans="4:4">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D74" s="7"/>
     </row>
-    <row r="75" spans="4:4">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D75" s="7"/>
     </row>
-    <row r="76" spans="4:4">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D76" s="7"/>
     </row>
-    <row r="77" spans="4:4">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D77" s="7"/>
     </row>
-    <row r="78" spans="4:4">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D78" s="7"/>
     </row>
-    <row r="79" spans="4:4">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D79" s="7"/>
     </row>
-    <row r="80" spans="4:4">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D80" s="7"/>
     </row>
-    <row r="81" spans="4:4">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D81" s="7"/>
     </row>
-    <row r="82" spans="4:4">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D82" s="7"/>
     </row>
-    <row r="83" spans="4:4">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D83" s="7"/>
     </row>
-    <row r="84" spans="4:4">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D84" s="7"/>
     </row>
-    <row r="85" spans="4:4">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D85" s="7"/>
     </row>
-    <row r="86" spans="4:4">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D86" s="7"/>
     </row>
-    <row r="87" spans="4:4">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D87" s="7"/>
     </row>
-    <row r="88" spans="4:4">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D88" s="7"/>
     </row>
-    <row r="89" spans="4:4">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D89" s="7"/>
     </row>
-    <row r="90" spans="4:4">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D90" s="7"/>
     </row>
-    <row r="91" spans="4:4">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D91" s="7"/>
     </row>
-    <row r="92" spans="4:4">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D92" s="7"/>
     </row>
-    <row r="93" spans="4:4">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D93" s="7"/>
     </row>
-    <row r="94" spans="4:4">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D94" s="7"/>
     </row>
-    <row r="95" spans="4:4">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D95" s="7"/>
     </row>
-    <row r="96" spans="4:4">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D96" s="7"/>
     </row>
-    <row r="97" spans="4:4">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D97" s="7"/>
     </row>
-    <row r="98" spans="4:4">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D98" s="7"/>
     </row>
-    <row r="100" spans="4:4">
-      <c r="D100" s="7"/>
-    </row>
-    <row r="101" spans="4:4">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D99" s="7"/>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D101" s="7"/>
     </row>
-    <row r="102" spans="4:4">
+    <row r="102" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D102" s="7"/>
     </row>
-    <row r="103" spans="4:4">
+    <row r="103" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D103" s="7"/>
     </row>
-    <row r="104" spans="4:4">
+    <row r="104" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D104" s="7"/>
     </row>
-    <row r="105" spans="4:4">
+    <row r="105" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D105" s="7"/>
     </row>
-    <row r="106" spans="4:4">
+    <row r="106" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D106" s="7"/>
     </row>
-    <row r="107" spans="4:4">
+    <row r="107" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D107" s="7"/>
     </row>
-    <row r="109" spans="4:4">
-      <c r="D109" s="7"/>
-    </row>
-    <row r="110" spans="4:4">
+    <row r="108" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D108" s="7"/>
+    </row>
+    <row r="110" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D110" s="7"/>
     </row>
-    <row r="111" spans="4:4">
+    <row r="111" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D111" s="7"/>
     </row>
-    <row r="112" spans="4:4">
+    <row r="112" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D112" s="7"/>
     </row>
-    <row r="113" spans="4:4">
+    <row r="113" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D113" s="7"/>
     </row>
-    <row r="114" spans="4:4">
+    <row r="114" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D114" s="7"/>
     </row>
-    <row r="115" spans="4:4">
+    <row r="115" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D115" s="7"/>
     </row>
-    <row r="116" spans="4:4">
+    <row r="116" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D116" s="7"/>
     </row>
-    <row r="117" spans="4:4">
+    <row r="117" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D117" s="7"/>
     </row>
-    <row r="118" spans="4:4">
+    <row r="118" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D118" s="7"/>
     </row>
-    <row r="119" spans="4:4">
+    <row r="119" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D119" s="7"/>
     </row>
-    <row r="120" spans="4:4">
+    <row r="120" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D120" s="7"/>
     </row>
-    <row r="121" spans="4:4">
+    <row r="121" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D121" s="7"/>
     </row>
-    <row r="122" spans="4:4">
+    <row r="122" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D122" s="7"/>
     </row>
-    <row r="123" spans="4:4">
+    <row r="123" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D123" s="7"/>
     </row>
-    <row r="124" spans="4:4">
+    <row r="124" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D124" s="7"/>
     </row>
-    <row r="125" spans="4:4">
+    <row r="125" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D125" s="7"/>
     </row>
-    <row r="126" spans="4:4">
+    <row r="126" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D126" s="7"/>
     </row>
-    <row r="127" spans="4:4">
+    <row r="127" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D127" s="7"/>
     </row>
-    <row r="129" spans="4:4">
-      <c r="D129" s="7"/>
-    </row>
-    <row r="130" spans="4:4">
+    <row r="128" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D128" s="7"/>
+    </row>
+    <row r="130" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D130" s="7"/>
     </row>
-    <row r="131" spans="4:4">
+    <row r="131" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D131" s="7"/>
     </row>
-    <row r="132" spans="4:4">
+    <row r="132" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D132" s="7"/>
     </row>
-    <row r="133" spans="4:4">
+    <row r="133" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D133" s="7"/>
     </row>
-    <row r="134" spans="4:4">
+    <row r="134" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D134" s="7"/>
     </row>
-    <row r="135" spans="4:4">
+    <row r="135" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D135" s="7"/>
     </row>
-    <row r="136" spans="4:4">
+    <row r="136" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D136" s="7"/>
     </row>
-    <row r="137" spans="4:4">
+    <row r="137" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D137" s="7"/>
     </row>
-    <row r="138" spans="4:4">
+    <row r="138" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D138" s="7"/>
     </row>
-    <row r="139" spans="4:4">
+    <row r="139" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D139" s="7"/>
     </row>
-    <row r="140" spans="4:4">
+    <row r="140" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D140" s="7"/>
     </row>
-    <row r="141" spans="4:4">
+    <row r="141" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D141" s="7"/>
     </row>
-    <row r="142" spans="4:4">
+    <row r="142" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D142" s="7"/>
     </row>
-    <row r="143" spans="4:4">
+    <row r="143" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D143" s="7"/>
     </row>
-    <row r="144" spans="4:4">
+    <row r="144" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D144" s="7"/>
     </row>
-    <row r="145" spans="4:4">
+    <row r="145" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D145" s="7"/>
     </row>
-    <row r="146" spans="4:4">
+    <row r="146" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D146" s="7"/>
     </row>
-    <row r="147" spans="4:4">
+    <row r="147" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D147" s="7"/>
     </row>
-    <row r="148" spans="4:4">
+    <row r="148" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D148" s="7"/>
     </row>
-    <row r="149" spans="4:4">
+    <row r="149" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D149" s="7"/>
     </row>
-    <row r="150" spans="4:4">
+    <row r="150" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D150" s="7"/>
     </row>
-    <row r="151" spans="4:4">
+    <row r="151" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D151" s="7"/>
     </row>
-    <row r="152" spans="4:4">
+    <row r="152" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D152" s="7"/>
     </row>
-    <row r="153" spans="4:4">
+    <row r="153" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D153" s="7"/>
     </row>
-    <row r="154" spans="4:4">
+    <row r="154" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D154" s="7"/>
     </row>
-    <row r="155" spans="4:4">
+    <row r="155" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D155" s="7"/>
     </row>
-    <row r="156" spans="4:4">
+    <row r="156" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D156" s="7"/>
     </row>
-    <row r="157" spans="4:4">
+    <row r="157" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D157" s="7"/>
     </row>
-    <row r="158" spans="4:4">
+    <row r="158" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D158" s="7"/>
     </row>
-    <row r="159" spans="4:4">
+    <row r="159" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D159" s="7"/>
     </row>
-    <row r="160" spans="4:4">
+    <row r="160" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D160" s="7"/>
     </row>
-    <row r="161" spans="1:4">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D161" s="7"/>
     </row>
-    <row r="162" spans="1:4">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D162" s="7"/>
     </row>
-    <row r="163" spans="1:4">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D163" s="7"/>
     </row>
-    <row r="164" spans="1:4">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D164" s="7"/>
     </row>
-    <row r="165" spans="1:4">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D165" s="7"/>
     </row>
-    <row r="166" spans="1:4">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D166" s="7"/>
     </row>
-    <row r="167" spans="1:4">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D167" s="7"/>
     </row>
-    <row r="168" spans="1:4">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D168" s="7"/>
     </row>
-    <row r="169" spans="1:4">
-      <c r="A169" s="10"/>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D169" s="7"/>
     </row>
-    <row r="170" spans="1:4">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A170" s="10"/>
       <c r="D170" s="7"/>
     </row>
-    <row r="171" spans="1:4">
-      <c r="A171" s="10"/>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D171" s="7"/>
     </row>
-    <row r="172" spans="1:4">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A172" s="10"/>
       <c r="D172" s="7"/>
     </row>
-    <row r="174" spans="1:4">
-      <c r="D174" s="7"/>
-    </row>
-    <row r="175" spans="1:4">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A173" s="10"/>
+      <c r="D173" s="7"/>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D175" s="7"/>
     </row>
-    <row r="176" spans="1:4">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D176" s="7"/>
     </row>
-    <row r="177" spans="4:4">
+    <row r="177" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D177" s="7"/>
     </row>
-    <row r="178" spans="4:4">
+    <row r="178" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D178" s="7"/>
     </row>
-    <row r="179" spans="4:4">
+    <row r="179" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D179" s="7"/>
     </row>
-    <row r="180" spans="4:4">
+    <row r="180" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D180" s="7"/>
     </row>
-    <row r="181" spans="4:4">
+    <row r="181" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D181" s="7"/>
     </row>
-    <row r="182" spans="4:4">
+    <row r="182" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D182" s="7"/>
     </row>
-    <row r="183" spans="4:4">
+    <row r="183" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D183" s="7"/>
     </row>
-    <row r="184" spans="4:4">
+    <row r="184" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D184" s="7"/>
     </row>
-    <row r="185" spans="4:4">
+    <row r="185" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D185" s="7"/>
     </row>
-    <row r="186" spans="4:4">
+    <row r="186" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D186" s="7"/>
     </row>
-    <row r="187" spans="4:4">
+    <row r="187" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D187" s="7"/>
     </row>
-    <row r="188" spans="4:4">
+    <row r="188" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D188" s="7"/>
     </row>
-    <row r="189" spans="4:4">
+    <row r="189" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D189" s="7"/>
     </row>
-    <row r="190" spans="4:4">
+    <row r="190" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D190" s="7"/>
     </row>
-    <row r="191" spans="4:4">
+    <row r="191" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D191" s="7"/>
     </row>
-    <row r="192" spans="4:4">
+    <row r="192" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D192" s="7"/>
     </row>
-    <row r="193" spans="4:4">
+    <row r="193" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D193" s="7"/>
     </row>
-    <row r="194" spans="4:4">
+    <row r="194" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D194" s="7"/>
     </row>
-    <row r="195" spans="4:4">
+    <row r="195" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D195" s="7"/>
     </row>
-    <row r="196" spans="4:4">
+    <row r="196" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D196" s="7"/>
     </row>
-    <row r="197" spans="4:4">
+    <row r="197" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D197" s="7"/>
     </row>
-    <row r="198" spans="4:4">
+    <row r="198" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D198" s="7"/>
     </row>
-    <row r="199" spans="4:4">
+    <row r="199" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D199" s="7"/>
     </row>
-    <row r="200" spans="4:4">
+    <row r="200" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D200" s="7"/>
     </row>
-    <row r="201" spans="4:4">
+    <row r="201" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D201" s="7"/>
     </row>
-    <row r="202" spans="4:4">
+    <row r="202" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D202" s="7"/>
     </row>
-    <row r="203" spans="4:4">
+    <row r="203" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D203" s="7"/>
     </row>
-    <row r="204" spans="4:4">
+    <row r="204" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D204" s="7"/>
     </row>
-    <row r="205" spans="4:4">
+    <row r="205" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D205" s="7"/>
     </row>
-    <row r="206" spans="4:4">
+    <row r="206" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D206" s="7"/>
     </row>
-    <row r="207" spans="4:4">
+    <row r="207" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D207" s="7"/>
     </row>
-    <row r="208" spans="4:4">
+    <row r="208" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D208" s="7"/>
     </row>
-    <row r="209" spans="4:4">
+    <row r="209" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D209" s="7"/>
     </row>
-    <row r="210" spans="4:4">
+    <row r="210" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D210" s="7"/>
     </row>
-    <row r="211" spans="4:4">
+    <row r="211" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D211" s="7"/>
     </row>
-    <row r="212" spans="4:4">
+    <row r="212" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D212" s="7"/>
     </row>
-    <row r="213" spans="4:4">
+    <row r="213" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D213" s="7"/>
     </row>
-    <row r="214" spans="4:4">
+    <row r="214" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D214" s="7"/>
     </row>
-    <row r="215" spans="4:4">
+    <row r="215" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D215" s="7"/>
     </row>
-    <row r="216" spans="4:4">
+    <row r="216" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D216" s="7"/>
     </row>
-    <row r="217" spans="4:4">
+    <row r="217" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D217" s="7"/>
     </row>
-    <row r="218" spans="4:4">
+    <row r="218" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D218" s="7"/>
     </row>
-    <row r="219" spans="4:4">
+    <row r="219" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D219" s="7"/>
     </row>
-    <row r="220" spans="4:4">
+    <row r="220" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D220" s="7"/>
     </row>
-    <row r="221" spans="4:4">
+    <row r="221" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D221" s="7"/>
     </row>
-    <row r="222" spans="4:4">
+    <row r="222" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D222" s="7"/>
     </row>
-    <row r="223" spans="4:4">
+    <row r="223" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D223" s="7"/>
     </row>
-    <row r="224" spans="4:4">
+    <row r="224" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D224" s="7"/>
     </row>
-    <row r="225" spans="4:4">
+    <row r="225" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D225" s="7"/>
     </row>
-    <row r="226" spans="4:4">
+    <row r="226" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D226" s="7"/>
     </row>
-    <row r="227" spans="4:4">
+    <row r="227" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D227" s="7"/>
     </row>
-    <row r="228" spans="4:4">
+    <row r="228" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D228" s="7"/>
     </row>
-    <row r="229" spans="4:4">
+    <row r="229" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D229" s="7"/>
     </row>
-    <row r="230" spans="4:4">
+    <row r="230" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D230" s="7"/>
     </row>
-    <row r="231" spans="4:4">
+    <row r="231" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D231" s="7"/>
     </row>
-    <row r="232" spans="4:4">
+    <row r="232" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D232" s="7"/>
     </row>
-    <row r="233" spans="4:4">
+    <row r="233" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D233" s="7"/>
     </row>
-    <row r="234" spans="4:4">
+    <row r="234" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D234" s="7"/>
     </row>
-    <row r="235" spans="4:4">
+    <row r="235" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D235" s="7"/>
     </row>
-    <row r="236" spans="4:4">
+    <row r="236" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D236" s="7"/>
     </row>
-    <row r="237" spans="4:4">
+    <row r="237" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D237" s="7"/>
     </row>
-    <row r="238" spans="4:4">
+    <row r="238" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D238" s="7"/>
     </row>
-    <row r="239" spans="4:4">
+    <row r="239" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D239" s="7"/>
     </row>
-    <row r="240" spans="4:4">
+    <row r="240" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D240" s="7"/>
     </row>
-    <row r="241" spans="4:4">
+    <row r="241" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D241" s="7"/>
     </row>
-    <row r="242" spans="4:4">
+    <row r="242" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D242" s="7"/>
     </row>
-    <row r="243" spans="4:4">
+    <row r="243" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D243" s="7"/>
     </row>
-    <row r="244" spans="4:4">
+    <row r="244" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D244" s="7"/>
     </row>
-    <row r="245" spans="4:4">
+    <row r="245" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D245" s="7"/>
     </row>
-    <row r="246" spans="4:4">
+    <row r="246" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D246" s="7"/>
     </row>
-    <row r="247" spans="4:4">
+    <row r="247" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D247" s="7"/>
     </row>
-    <row r="248" spans="4:4">
+    <row r="248" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D248" s="7"/>
     </row>
-    <row r="249" spans="4:4">
+    <row r="249" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D249" s="7"/>
     </row>
-    <row r="250" spans="4:4">
+    <row r="250" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D250" s="7"/>
     </row>
-    <row r="251" spans="4:4">
+    <row r="251" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D251" s="7"/>
     </row>
-    <row r="252" spans="4:4">
+    <row r="252" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D252" s="7"/>
     </row>
-    <row r="253" spans="4:4">
+    <row r="253" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D253" s="7"/>
     </row>
-    <row r="254" spans="4:4">
+    <row r="254" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D254" s="7"/>
     </row>
-    <row r="255" spans="4:4">
+    <row r="255" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D255" s="7"/>
     </row>
-    <row r="256" spans="4:4">
+    <row r="256" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D256" s="7"/>
     </row>
-    <row r="257" spans="4:4">
+    <row r="257" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D257" s="7"/>
     </row>
-    <row r="258" spans="4:4">
+    <row r="258" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D258" s="7"/>
     </row>
-    <row r="259" spans="4:4">
+    <row r="259" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D259" s="7"/>
     </row>
-    <row r="260" spans="4:4">
+    <row r="260" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D260" s="7"/>
     </row>
-    <row r="261" spans="4:4">
+    <row r="261" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D261" s="7"/>
     </row>
-    <row r="262" spans="4:4">
+    <row r="262" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D262" s="7"/>
     </row>
-    <row r="263" spans="4:4">
+    <row r="263" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D263" s="7"/>
     </row>
-    <row r="264" spans="4:4">
+    <row r="264" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D264" s="7"/>
     </row>
-    <row r="265" spans="4:4">
+    <row r="265" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D265" s="7"/>
     </row>
-    <row r="266" spans="4:4">
+    <row r="266" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D266" s="7"/>
     </row>
-    <row r="267" spans="4:4">
+    <row r="267" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D267" s="7"/>
     </row>
-    <row r="268" spans="4:4">
+    <row r="268" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D268" s="7"/>
     </row>
-    <row r="269" spans="4:4">
+    <row r="269" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D269" s="7"/>
     </row>
-    <row r="270" spans="4:4">
+    <row r="270" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D270" s="7"/>
     </row>
-    <row r="271" spans="4:4">
+    <row r="271" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D271" s="7"/>
     </row>
-    <row r="272" spans="4:4">
+    <row r="272" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D272" s="7"/>
     </row>
-    <row r="273" spans="4:4">
+    <row r="273" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D273" s="7"/>
     </row>
-    <row r="274" spans="4:4">
+    <row r="274" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D274" s="7"/>
     </row>
-    <row r="275" spans="4:4">
+    <row r="275" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D275" s="7"/>
     </row>
-    <row r="276" spans="4:4">
+    <row r="276" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D276" s="7"/>
     </row>
-    <row r="277" spans="4:4">
+    <row r="277" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D277" s="7"/>
     </row>
-    <row r="278" spans="4:4">
+    <row r="278" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D278" s="7"/>
     </row>
-    <row r="279" spans="4:4">
+    <row r="279" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D279" s="7"/>
     </row>
-    <row r="280" spans="4:4">
+    <row r="280" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D280" s="7"/>
     </row>
-    <row r="281" spans="4:4">
+    <row r="281" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D281" s="7"/>
     </row>
-    <row r="282" spans="4:4">
+    <row r="282" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D282" s="7"/>
     </row>
-    <row r="283" spans="4:4">
+    <row r="283" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D283" s="7"/>
     </row>
-    <row r="284" spans="4:4">
+    <row r="284" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D284" s="7"/>
     </row>
-    <row r="285" spans="4:4">
+    <row r="285" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D285" s="7"/>
     </row>
-    <row r="286" spans="4:4">
+    <row r="286" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D286" s="7"/>
     </row>
-    <row r="287" spans="4:4">
+    <row r="287" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D287" s="7"/>
     </row>
-    <row r="288" spans="4:4">
+    <row r="288" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D288" s="7"/>
     </row>
-    <row r="289" spans="4:4">
+    <row r="289" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D289" s="7"/>
     </row>
-    <row r="290" spans="4:4">
+    <row r="290" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D290" s="7"/>
     </row>
-    <row r="291" spans="4:4">
+    <row r="291" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D291" s="7"/>
     </row>
-    <row r="292" spans="4:4">
+    <row r="292" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D292" s="7"/>
     </row>
-    <row r="293" spans="4:4">
+    <row r="293" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D293" s="7"/>
     </row>
-    <row r="294" spans="4:4">
+    <row r="294" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D294" s="7"/>
     </row>
-    <row r="295" spans="4:4">
+    <row r="295" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D295" s="7"/>
     </row>
-    <row r="296" spans="4:4">
+    <row r="296" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D296" s="7"/>
     </row>
-    <row r="297" spans="4:4">
+    <row r="297" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D297" s="7"/>
     </row>
-    <row r="298" spans="4:4">
+    <row r="298" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D298" s="7"/>
     </row>
-    <row r="299" spans="4:4">
+    <row r="299" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D299" s="7"/>
     </row>
-    <row r="300" spans="4:4">
+    <row r="300" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D300" s="7"/>
     </row>
-    <row r="301" spans="4:4">
+    <row r="301" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D301" s="7"/>
     </row>
-    <row r="302" spans="4:4">
+    <row r="302" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D302" s="7"/>
     </row>
-    <row r="303" spans="4:4">
+    <row r="303" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D303" s="7"/>
     </row>
-    <row r="304" spans="4:4">
+    <row r="304" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D304" s="7"/>
     </row>
-    <row r="305" spans="4:4">
+    <row r="305" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D305" s="7"/>
     </row>
-    <row r="306" spans="4:4">
+    <row r="306" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D306" s="7"/>
     </row>
-    <row r="307" spans="4:4">
+    <row r="307" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D307" s="7"/>
     </row>
-    <row r="308" spans="4:4">
+    <row r="308" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D308" s="7"/>
     </row>
-    <row r="309" spans="4:4">
+    <row r="309" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D309" s="7"/>
     </row>
-    <row r="310" spans="4:4">
+    <row r="310" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D310" s="7"/>
     </row>
-    <row r="311" spans="4:4">
+    <row r="311" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D311" s="7"/>
     </row>
-    <row r="312" spans="4:4">
+    <row r="312" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D312" s="7"/>
     </row>
-    <row r="313" spans="4:4">
+    <row r="313" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D313" s="7"/>
     </row>
-    <row r="314" spans="4:4">
+    <row r="314" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D314" s="7"/>
     </row>
-    <row r="315" spans="4:4">
+    <row r="315" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D315" s="7"/>
     </row>
-    <row r="316" spans="4:4">
+    <row r="316" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D316" s="7"/>
     </row>
-    <row r="317" spans="4:4">
+    <row r="317" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D317" s="7"/>
     </row>
-    <row r="318" spans="4:4">
+    <row r="318" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D318" s="7"/>
     </row>
-    <row r="319" spans="4:4">
+    <row r="319" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D319" s="7"/>
     </row>
-    <row r="320" spans="4:4">
+    <row r="320" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D320" s="7"/>
     </row>
-    <row r="321" spans="4:4">
+    <row r="321" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D321" s="7"/>
     </row>
-    <row r="322" spans="4:4">
+    <row r="322" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D322" s="7"/>
     </row>
-    <row r="323" spans="4:4">
+    <row r="323" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D323" s="7"/>
     </row>
-    <row r="324" spans="4:4">
+    <row r="324" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D324" s="7"/>
     </row>
-    <row r="325" spans="4:4">
+    <row r="325" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D325" s="7"/>
     </row>
-    <row r="326" spans="4:4">
+    <row r="326" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D326" s="7"/>
     </row>
-    <row r="327" spans="4:4">
+    <row r="327" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D327" s="7"/>
     </row>
-    <row r="328" spans="4:4">
+    <row r="328" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D328" s="7"/>
     </row>
-    <row r="329" spans="4:4">
+    <row r="329" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D329" s="7"/>
     </row>
-    <row r="330" spans="4:4">
+    <row r="330" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D330" s="7"/>
     </row>
-    <row r="331" spans="4:4">
+    <row r="331" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D331" s="7"/>
     </row>
-    <row r="332" spans="4:4">
+    <row r="332" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D332" s="7"/>
     </row>
-    <row r="333" spans="4:4">
+    <row r="333" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D333" s="7"/>
     </row>
-    <row r="334" spans="4:4">
+    <row r="334" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D334" s="7"/>
     </row>
-    <row r="335" spans="4:4">
+    <row r="335" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D335" s="7"/>
     </row>
-    <row r="336" spans="4:4">
+    <row r="336" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D336" s="7"/>
     </row>
-    <row r="337" spans="4:4">
+    <row r="337" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D337" s="7"/>
     </row>
-    <row r="338" spans="4:4">
+    <row r="338" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D338" s="7"/>
     </row>
-    <row r="339" spans="4:4">
+    <row r="339" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D339" s="7"/>
     </row>
-    <row r="340" spans="4:4">
+    <row r="340" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D340" s="7"/>
     </row>
-    <row r="341" spans="4:4">
+    <row r="341" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D341" s="7"/>
+    </row>
+    <row r="342" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D342" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>